<commit_message>
Changes in Excel File
</commit_message>
<xml_diff>
--- a/FINAL450 Qs for DS ALGo.xlsx
+++ b/FINAL450 Qs for DS ALGo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python Learning Plus\PROGRAMS\Coding Ninjas DS Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE42E82D-D62B-4F04-BD84-A71F68332A54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62C8D14-8BD1-4A1E-8332-B7A7712AF868}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1429,7 +1429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1498,8 +1498,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1517,6 +1532,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1527,12 +1547,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1553,17 +1574,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1879,7 +1904,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1898,6 +1923,10 @@
       <c r="B2" s="8" t="s">
         <v>464</v>
       </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="21">
       <c r="A4" s="2" t="s">
@@ -1906,7 +1935,7 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1922,7 +1951,7 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1933,7 +1962,7 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1945,7 +1974,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1955,7 +1984,7 @@
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1966,7 +1995,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1977,7 +2006,7 @@
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1988,7 +2017,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1999,7 +2028,7 @@
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2010,7 +2039,7 @@
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2021,7 +2050,7 @@
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2032,7 +2061,7 @@
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2043,7 +2072,7 @@
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2054,7 +2083,7 @@
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2065,7 +2094,7 @@
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2076,7 +2105,7 @@
       <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2087,7 +2116,7 @@
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2098,7 +2127,7 @@
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2109,7 +2138,7 @@
       <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2120,7 +2149,7 @@
       <c r="B24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2131,7 +2160,7 @@
       <c r="B25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2142,7 +2171,7 @@
       <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2153,7 +2182,7 @@
       <c r="B27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2164,7 +2193,7 @@
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2175,7 +2204,7 @@
       <c r="B29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2186,7 +2215,7 @@
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2197,7 +2226,7 @@
       <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2208,7 +2237,7 @@
       <c r="B32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2219,7 +2248,7 @@
       <c r="B33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2230,7 +2259,7 @@
       <c r="B34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2241,7 +2270,7 @@
       <c r="B35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2252,7 +2281,7 @@
       <c r="B36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2263,7 +2292,7 @@
       <c r="B37" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2274,7 +2303,7 @@
       <c r="B38" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2285,7 +2314,7 @@
       <c r="B39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2296,7 +2325,7 @@
       <c r="B40" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2307,20 +2336,20 @@
       <c r="B41" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">
       <c r="B42" s="5"/>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="21">
       <c r="A43" s="3"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2331,7 +2360,7 @@
       <c r="B44" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2342,7 +2371,7 @@
       <c r="B45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2353,7 +2382,7 @@
       <c r="B46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2364,7 +2393,7 @@
       <c r="B47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2375,7 +2404,7 @@
       <c r="B48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2386,7 +2415,7 @@
       <c r="B49" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2397,7 +2426,7 @@
       <c r="B50" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2408,7 +2437,7 @@
       <c r="B51" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2419,7 +2448,7 @@
       <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2430,14 +2459,14 @@
       <c r="B53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">
       <c r="A55" s="3"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="11"/>
+      <c r="C55" s="10"/>
     </row>
     <row r="56" spans="1:3" ht="21">
       <c r="A56" s="3" t="s">
@@ -2446,7 +2475,7 @@
       <c r="B56" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2457,7 +2486,7 @@
       <c r="B57" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2468,7 +2497,7 @@
       <c r="B58" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2479,7 +2508,7 @@
       <c r="B59" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2490,7 +2519,7 @@
       <c r="B60" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2501,7 +2530,7 @@
       <c r="B61" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2512,7 +2541,7 @@
       <c r="B62" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2523,7 +2552,7 @@
       <c r="B63" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2534,7 +2563,7 @@
       <c r="B64" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2545,7 +2574,7 @@
       <c r="B65" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2556,7 +2585,7 @@
       <c r="B66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2567,7 +2596,7 @@
       <c r="B67" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2578,7 +2607,7 @@
       <c r="B68" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2589,7 +2618,7 @@
       <c r="B69" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2600,7 +2629,7 @@
       <c r="B70" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2611,7 +2640,7 @@
       <c r="B71" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2622,7 +2651,7 @@
       <c r="B72" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2633,7 +2662,7 @@
       <c r="B73" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2644,7 +2673,7 @@
       <c r="B74" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2655,7 +2684,7 @@
       <c r="B75" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2666,7 +2695,7 @@
       <c r="B76" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2677,7 +2706,7 @@
       <c r="B77" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2688,7 +2717,7 @@
       <c r="B78" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2699,7 +2728,7 @@
       <c r="B79" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2710,7 +2739,7 @@
       <c r="B80" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C80" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2721,7 +2750,7 @@
       <c r="B81" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2732,7 +2761,7 @@
       <c r="B82" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2743,7 +2772,7 @@
       <c r="B83" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2754,7 +2783,7 @@
       <c r="B84" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2765,7 +2794,7 @@
       <c r="B85" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2776,7 +2805,7 @@
       <c r="B86" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2787,7 +2816,7 @@
       <c r="B87" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C87" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2798,7 +2827,7 @@
       <c r="B88" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2809,7 +2838,7 @@
       <c r="B89" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2820,7 +2849,7 @@
       <c r="B90" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2831,7 +2860,7 @@
       <c r="B91" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2842,7 +2871,7 @@
       <c r="B92" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2853,7 +2882,7 @@
       <c r="B93" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2864,7 +2893,7 @@
       <c r="B94" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2875,7 +2904,7 @@
       <c r="B95" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2886,7 +2915,7 @@
       <c r="B96" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2897,7 +2926,7 @@
       <c r="B97" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2908,14 +2937,14 @@
       <c r="B98" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="21">
       <c r="A100" s="6"/>
       <c r="B100" s="5"/>
-      <c r="C100" s="11"/>
+      <c r="C100" s="10"/>
     </row>
     <row r="101" spans="1:3" ht="21">
       <c r="A101" s="3" t="s">
@@ -2924,7 +2953,7 @@
       <c r="B101" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2935,7 +2964,7 @@
       <c r="B102" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2946,7 +2975,7 @@
       <c r="B103" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2957,7 +2986,7 @@
       <c r="B104" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2968,7 +2997,7 @@
       <c r="B105" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2979,7 +3008,7 @@
       <c r="B106" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2990,7 +3019,7 @@
       <c r="B107" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3001,7 +3030,7 @@
       <c r="B108" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3012,7 +3041,7 @@
       <c r="B109" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3023,7 +3052,7 @@
       <c r="B110" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3034,7 +3063,7 @@
       <c r="B111" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3045,7 +3074,7 @@
       <c r="B112" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3056,7 +3085,7 @@
       <c r="B113" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3067,7 +3096,7 @@
       <c r="B114" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3078,7 +3107,7 @@
       <c r="B115" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3089,7 +3118,7 @@
       <c r="B116" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3100,7 +3129,7 @@
       <c r="B117" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3111,7 +3140,7 @@
       <c r="B118" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3122,7 +3151,7 @@
       <c r="B119" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3133,7 +3162,7 @@
       <c r="B120" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3144,7 +3173,7 @@
       <c r="B121" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3155,7 +3184,7 @@
       <c r="B122" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C122" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3166,7 +3195,7 @@
       <c r="B123" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3177,7 +3206,7 @@
       <c r="B124" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C124" s="11" t="s">
+      <c r="C124" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3188,7 +3217,7 @@
       <c r="B125" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="11" t="s">
+      <c r="C125" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3199,7 +3228,7 @@
       <c r="B126" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C126" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3210,7 +3239,7 @@
       <c r="B127" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C127" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3221,7 +3250,7 @@
       <c r="B128" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C128" s="11" t="s">
+      <c r="C128" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3232,7 +3261,7 @@
       <c r="B129" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C129" s="11" t="s">
+      <c r="C129" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3243,7 +3272,7 @@
       <c r="B130" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C130" s="11" t="s">
+      <c r="C130" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3254,7 +3283,7 @@
       <c r="B131" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C131" s="11" t="s">
+      <c r="C131" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3265,7 +3294,7 @@
       <c r="B132" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C132" s="11" t="s">
+      <c r="C132" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3276,7 +3305,7 @@
       <c r="B133" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3287,7 +3316,7 @@
       <c r="B134" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C134" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3298,7 +3327,7 @@
       <c r="B135" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3309,13 +3338,13 @@
       <c r="B136" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="21">
       <c r="B138" s="5"/>
-      <c r="C138" s="11"/>
+      <c r="C138" s="10"/>
     </row>
     <row r="139" spans="1:3" ht="21">
       <c r="A139" s="6" t="s">
@@ -3324,7 +3353,7 @@
       <c r="B139" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C139" s="11" t="s">
+      <c r="C139" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3335,7 +3364,7 @@
       <c r="B140" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C140" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3346,7 +3375,7 @@
       <c r="B141" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C141" s="11" t="s">
+      <c r="C141" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3357,7 +3386,7 @@
       <c r="B142" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="C142" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3368,7 +3397,7 @@
       <c r="B143" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C143" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3379,7 +3408,7 @@
       <c r="B144" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C144" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3390,7 +3419,7 @@
       <c r="B145" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3401,7 +3430,7 @@
       <c r="B146" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C146" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3412,7 +3441,7 @@
       <c r="B147" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C147" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3423,7 +3452,7 @@
       <c r="B148" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C148" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3434,7 +3463,7 @@
       <c r="B149" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="C149" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3445,7 +3474,7 @@
       <c r="B150" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C150" s="11" t="s">
+      <c r="C150" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3456,7 +3485,7 @@
       <c r="B151" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="C151" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3467,7 +3496,7 @@
       <c r="B152" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C152" s="11" t="s">
+      <c r="C152" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3478,7 +3507,7 @@
       <c r="B153" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C153" s="11" t="s">
+      <c r="C153" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3489,7 +3518,7 @@
       <c r="B154" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C154" s="11" t="s">
+      <c r="C154" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3500,7 +3529,7 @@
       <c r="B155" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="C155" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3511,7 +3540,7 @@
       <c r="B156" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="C156" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3522,7 +3551,7 @@
       <c r="B157" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C157" s="11" t="s">
+      <c r="C157" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3533,7 +3562,7 @@
       <c r="B158" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="C158" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3544,7 +3573,7 @@
       <c r="B159" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C159" s="11" t="s">
+      <c r="C159" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3555,7 +3584,7 @@
       <c r="B160" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C160" s="11" t="s">
+      <c r="C160" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3566,7 +3595,7 @@
       <c r="B161" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C161" s="11" t="s">
+      <c r="C161" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3577,7 +3606,7 @@
       <c r="B162" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C162" s="11" t="s">
+      <c r="C162" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3588,7 +3617,7 @@
       <c r="B163" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C163" s="11" t="s">
+      <c r="C163" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3599,7 +3628,7 @@
       <c r="B164" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C164" s="11" t="s">
+      <c r="C164" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3610,7 +3639,7 @@
       <c r="B165" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C165" s="11" t="s">
+      <c r="C165" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3621,7 +3650,7 @@
       <c r="B166" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C166" s="11" t="s">
+      <c r="C166" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3632,7 +3661,7 @@
       <c r="B167" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C167" s="11" t="s">
+      <c r="C167" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3643,7 +3672,7 @@
       <c r="B168" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C168" s="11" t="s">
+      <c r="C168" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3654,7 +3683,7 @@
       <c r="B169" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C169" s="11" t="s">
+      <c r="C169" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3665,7 +3694,7 @@
       <c r="B170" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C170" s="11" t="s">
+      <c r="C170" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3676,7 +3705,7 @@
       <c r="B171" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C171" s="11" t="s">
+      <c r="C171" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3687,7 +3716,7 @@
       <c r="B172" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C172" s="11" t="s">
+      <c r="C172" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3698,7 +3727,7 @@
       <c r="B173" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C173" s="11" t="s">
+      <c r="C173" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3709,13 +3738,13 @@
       <c r="B174" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C174" s="11" t="s">
+      <c r="C174" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="21">
       <c r="B176" s="5"/>
-      <c r="C176" s="11"/>
+      <c r="C176" s="10"/>
     </row>
     <row r="177" spans="1:3" ht="21">
       <c r="A177" s="3" t="s">
@@ -3724,7 +3753,7 @@
       <c r="B177" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C177" s="11" t="s">
+      <c r="C177" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3735,7 +3764,7 @@
       <c r="B178" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C178" s="11" t="s">
+      <c r="C178" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3746,7 +3775,7 @@
       <c r="B179" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C179" s="11" t="s">
+      <c r="C179" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3757,7 +3786,7 @@
       <c r="B180" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C180" s="11" t="s">
+      <c r="C180" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3768,7 +3797,7 @@
       <c r="B181" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C181" s="11" t="s">
+      <c r="C181" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3779,7 +3808,7 @@
       <c r="B182" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C182" s="11" t="s">
+      <c r="C182" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3790,7 +3819,7 @@
       <c r="B183" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C183" s="11" t="s">
+      <c r="C183" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3801,7 +3830,7 @@
       <c r="B184" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C184" s="11" t="s">
+      <c r="C184" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3812,7 +3841,7 @@
       <c r="B185" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C185" s="11" t="s">
+      <c r="C185" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3823,7 +3852,7 @@
       <c r="B186" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="11" t="s">
+      <c r="C186" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3834,7 +3863,7 @@
       <c r="B187" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C187" s="11" t="s">
+      <c r="C187" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3845,7 +3874,7 @@
       <c r="B188" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C188" s="11" t="s">
+      <c r="C188" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3856,7 +3885,7 @@
       <c r="B189" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C189" s="11" t="s">
+      <c r="C189" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3867,7 +3896,7 @@
       <c r="B190" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C190" s="11" t="s">
+      <c r="C190" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3878,7 +3907,7 @@
       <c r="B191" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C191" s="11" t="s">
+      <c r="C191" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3889,7 +3918,7 @@
       <c r="B192" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C192" s="11" t="s">
+      <c r="C192" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3900,7 +3929,7 @@
       <c r="B193" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C193" s="11" t="s">
+      <c r="C193" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3911,7 +3940,7 @@
       <c r="B194" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C194" s="11" t="s">
+      <c r="C194" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3922,7 +3951,7 @@
       <c r="B195" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C195" s="11" t="s">
+      <c r="C195" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3933,7 +3962,7 @@
       <c r="B196" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C196" s="11" t="s">
+      <c r="C196" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3944,7 +3973,7 @@
       <c r="B197" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C197" s="11" t="s">
+      <c r="C197" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3955,7 +3984,7 @@
       <c r="B198" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C198" s="11" t="s">
+      <c r="C198" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3966,7 +3995,7 @@
       <c r="B199" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C199" s="11" t="s">
+      <c r="C199" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3977,7 +4006,7 @@
       <c r="B200" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C200" s="11" t="s">
+      <c r="C200" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3988,7 +4017,7 @@
       <c r="B201" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C201" s="11" t="s">
+      <c r="C201" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3999,7 +4028,7 @@
       <c r="B202" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C202" s="11" t="s">
+      <c r="C202" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4010,7 +4039,7 @@
       <c r="B203" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C203" s="11" t="s">
+      <c r="C203" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4021,7 +4050,7 @@
       <c r="B204" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C204" s="11" t="s">
+      <c r="C204" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4032,7 +4061,7 @@
       <c r="B205" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C205" s="11" t="s">
+      <c r="C205" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4043,7 +4072,7 @@
       <c r="B206" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C206" s="11" t="s">
+      <c r="C206" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4054,7 +4083,7 @@
       <c r="B207" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C207" s="11" t="s">
+      <c r="C207" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4065,7 +4094,7 @@
       <c r="B208" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C208" s="11" t="s">
+      <c r="C208" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4076,7 +4105,7 @@
       <c r="B209" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C209" s="11" t="s">
+      <c r="C209" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4087,7 +4116,7 @@
       <c r="B210" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C210" s="11" t="s">
+      <c r="C210" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4098,19 +4127,19 @@
       <c r="B211" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C211" s="11" t="s">
+      <c r="C211" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">
       <c r="A212" s="6"/>
       <c r="B212" s="5"/>
-      <c r="C212" s="11"/>
+      <c r="C212" s="10"/>
     </row>
     <row r="213" spans="1:3" ht="21">
       <c r="A213" s="6"/>
       <c r="B213" s="5"/>
-      <c r="C213" s="11"/>
+      <c r="C213" s="10"/>
     </row>
     <row r="214" spans="1:3" ht="21">
       <c r="A214" s="3" t="s">
@@ -4119,7 +4148,7 @@
       <c r="B214" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C214" s="11" t="s">
+      <c r="C214" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4130,7 +4159,7 @@
       <c r="B215" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C215" s="11" t="s">
+      <c r="C215" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4141,7 +4170,7 @@
       <c r="B216" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C216" s="11" t="s">
+      <c r="C216" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4152,7 +4181,7 @@
       <c r="B217" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C217" s="11" t="s">
+      <c r="C217" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4163,7 +4192,7 @@
       <c r="B218" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C218" s="11" t="s">
+      <c r="C218" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4174,7 +4203,7 @@
       <c r="B219" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C219" s="11" t="s">
+      <c r="C219" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4185,7 +4214,7 @@
       <c r="B220" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C220" s="11" t="s">
+      <c r="C220" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4196,7 +4225,7 @@
       <c r="B221" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C221" s="11" t="s">
+      <c r="C221" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4207,7 +4236,7 @@
       <c r="B222" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C222" s="11" t="s">
+      <c r="C222" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4218,7 +4247,7 @@
       <c r="B223" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C223" s="11" t="s">
+      <c r="C223" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4229,7 +4258,7 @@
       <c r="B224" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C224" s="11" t="s">
+      <c r="C224" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4240,7 +4269,7 @@
       <c r="B225" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C225" s="11" t="s">
+      <c r="C225" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4251,7 +4280,7 @@
       <c r="B226" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C226" s="11" t="s">
+      <c r="C226" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4262,7 +4291,7 @@
       <c r="B227" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C227" s="11" t="s">
+      <c r="C227" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4273,7 +4302,7 @@
       <c r="B228" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C228" s="11" t="s">
+      <c r="C228" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4284,7 +4313,7 @@
       <c r="B229" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C229" s="11" t="s">
+      <c r="C229" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4295,7 +4324,7 @@
       <c r="B230" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C230" s="11" t="s">
+      <c r="C230" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4306,7 +4335,7 @@
       <c r="B231" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="C231" s="11" t="s">
+      <c r="C231" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4317,7 +4346,7 @@
       <c r="B232" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="C232" s="11" t="s">
+      <c r="C232" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4328,7 +4357,7 @@
       <c r="B233" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C233" s="11" t="s">
+      <c r="C233" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4339,7 +4368,7 @@
       <c r="B234" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C234" s="11" t="s">
+      <c r="C234" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4350,17 +4379,17 @@
       <c r="B235" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C235" s="11" t="s">
+      <c r="C235" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">
       <c r="B236" s="5"/>
-      <c r="C236" s="11"/>
+      <c r="C236" s="10"/>
     </row>
     <row r="237" spans="1:3" ht="21">
       <c r="B237" s="5"/>
-      <c r="C237" s="11"/>
+      <c r="C237" s="10"/>
     </row>
     <row r="238" spans="1:3" ht="21">
       <c r="A238" s="3" t="s">
@@ -4369,7 +4398,7 @@
       <c r="B238" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C238" s="11" t="s">
+      <c r="C238" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4380,7 +4409,7 @@
       <c r="B239" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C239" s="11" t="s">
+      <c r="C239" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4391,7 +4420,7 @@
       <c r="B240" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C240" s="11" t="s">
+      <c r="C240" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4402,7 +4431,7 @@
       <c r="B241" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C241" s="11" t="s">
+      <c r="C241" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4413,7 +4442,7 @@
       <c r="B242" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C242" s="11" t="s">
+      <c r="C242" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4424,7 +4453,7 @@
       <c r="B243" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C243" s="11" t="s">
+      <c r="C243" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4435,7 +4464,7 @@
       <c r="B244" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C244" s="11" t="s">
+      <c r="C244" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4446,7 +4475,7 @@
       <c r="B245" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C245" s="11" t="s">
+      <c r="C245" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4457,7 +4486,7 @@
       <c r="B246" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="C246" s="11" t="s">
+      <c r="C246" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4468,7 +4497,7 @@
       <c r="B247" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C247" s="11" t="s">
+      <c r="C247" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4479,7 +4508,7 @@
       <c r="B248" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C248" s="11" t="s">
+      <c r="C248" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4490,7 +4519,7 @@
       <c r="B249" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C249" s="11" t="s">
+      <c r="C249" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4501,7 +4530,7 @@
       <c r="B250" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C250" s="11" t="s">
+      <c r="C250" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4512,7 +4541,7 @@
       <c r="B251" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C251" s="11" t="s">
+      <c r="C251" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4523,7 +4552,7 @@
       <c r="B252" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C252" s="11" t="s">
+      <c r="C252" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4534,7 +4563,7 @@
       <c r="B253" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C253" s="11" t="s">
+      <c r="C253" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4545,7 +4574,7 @@
       <c r="B254" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C254" s="11" t="s">
+      <c r="C254" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4556,7 +4585,7 @@
       <c r="B255" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C255" s="11" t="s">
+      <c r="C255" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4567,7 +4596,7 @@
       <c r="B256" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C256" s="11" t="s">
+      <c r="C256" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4578,7 +4607,7 @@
       <c r="B257" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C257" s="11" t="s">
+      <c r="C257" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4589,7 +4618,7 @@
       <c r="B258" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="C258" s="11" t="s">
+      <c r="C258" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4600,7 +4629,7 @@
       <c r="B259" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C259" s="11" t="s">
+      <c r="C259" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4611,7 +4640,7 @@
       <c r="B260" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C260" s="11" t="s">
+      <c r="C260" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4622,7 +4651,7 @@
       <c r="B261" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C261" s="11" t="s">
+      <c r="C261" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4633,7 +4662,7 @@
       <c r="B262" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C262" s="11" t="s">
+      <c r="C262" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4644,7 +4673,7 @@
       <c r="B263" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C263" s="11" t="s">
+      <c r="C263" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4655,7 +4684,7 @@
       <c r="B264" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C264" s="11" t="s">
+      <c r="C264" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4666,7 +4695,7 @@
       <c r="B265" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C265" s="11" t="s">
+      <c r="C265" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4677,7 +4706,7 @@
       <c r="B266" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="C266" s="11" t="s">
+      <c r="C266" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4688,7 +4717,7 @@
       <c r="B267" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C267" s="11" t="s">
+      <c r="C267" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4699,7 +4728,7 @@
       <c r="B268" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C268" s="11" t="s">
+      <c r="C268" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4710,7 +4739,7 @@
       <c r="B269" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C269" s="11" t="s">
+      <c r="C269" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4721,7 +4750,7 @@
       <c r="B270" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C270" s="11" t="s">
+      <c r="C270" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4732,7 +4761,7 @@
       <c r="B271" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C271" s="11" t="s">
+      <c r="C271" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4743,17 +4772,17 @@
       <c r="B272" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C272" s="11" t="s">
+      <c r="C272" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="21">
       <c r="B273" s="5"/>
-      <c r="C273" s="11"/>
+      <c r="C273" s="10"/>
     </row>
     <row r="274" spans="1:3" ht="21">
       <c r="B274" s="5"/>
-      <c r="C274" s="11"/>
+      <c r="C274" s="10"/>
     </row>
     <row r="275" spans="1:3" ht="21">
       <c r="A275" s="3" t="s">
@@ -4762,7 +4791,7 @@
       <c r="B275" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C275" s="11" t="s">
+      <c r="C275" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4773,7 +4802,7 @@
       <c r="B276" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="C276" s="11" t="s">
+      <c r="C276" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4784,7 +4813,7 @@
       <c r="B277" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C277" s="11" t="s">
+      <c r="C277" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4795,7 +4824,7 @@
       <c r="B278" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="C278" s="11" t="s">
+      <c r="C278" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4806,7 +4835,7 @@
       <c r="B279" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C279" s="11" t="s">
+      <c r="C279" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4817,7 +4846,7 @@
       <c r="B280" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C280" s="11" t="s">
+      <c r="C280" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4828,7 +4857,7 @@
       <c r="B281" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C281" s="11" t="s">
+      <c r="C281" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4839,7 +4868,7 @@
       <c r="B282" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C282" s="11" t="s">
+      <c r="C282" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4850,7 +4879,7 @@
       <c r="B283" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C283" s="11" t="s">
+      <c r="C283" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4861,7 +4890,7 @@
       <c r="B284" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C284" s="11" t="s">
+      <c r="C284" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4872,7 +4901,7 @@
       <c r="B285" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C285" s="11" t="s">
+      <c r="C285" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4883,7 +4912,7 @@
       <c r="B286" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C286" s="11" t="s">
+      <c r="C286" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4894,7 +4923,7 @@
       <c r="B287" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="C287" s="11" t="s">
+      <c r="C287" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4905,7 +4934,7 @@
       <c r="B288" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C288" s="11" t="s">
+      <c r="C288" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4916,7 +4945,7 @@
       <c r="B289" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C289" s="11" t="s">
+      <c r="C289" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4927,7 +4956,7 @@
       <c r="B290" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="C290" s="11" t="s">
+      <c r="C290" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4938,7 +4967,7 @@
       <c r="B291" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C291" s="11" t="s">
+      <c r="C291" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4949,7 +4978,7 @@
       <c r="B292" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="C292" s="11" t="s">
+      <c r="C292" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4960,17 +4989,17 @@
       <c r="B293" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C293" s="11" t="s">
+      <c r="C293" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="21">
       <c r="B294" s="5"/>
-      <c r="C294" s="11"/>
+      <c r="C294" s="10"/>
     </row>
     <row r="295" spans="1:3" ht="21">
       <c r="B295" s="5"/>
-      <c r="C295" s="11"/>
+      <c r="C295" s="10"/>
     </row>
     <row r="296" spans="1:3" ht="21">
       <c r="A296" s="3" t="s">
@@ -4979,7 +5008,7 @@
       <c r="B296" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="C296" s="11" t="s">
+      <c r="C296" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4990,7 +5019,7 @@
       <c r="B297" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C297" s="11" t="s">
+      <c r="C297" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5001,7 +5030,7 @@
       <c r="B298" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C298" s="11" t="s">
+      <c r="C298" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5012,7 +5041,7 @@
       <c r="B299" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C299" s="11" t="s">
+      <c r="C299" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5023,7 +5052,7 @@
       <c r="B300" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C300" s="11" t="s">
+      <c r="C300" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5034,7 +5063,7 @@
       <c r="B301" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C301" s="11" t="s">
+      <c r="C301" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5045,7 +5074,7 @@
       <c r="B302" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C302" s="11" t="s">
+      <c r="C302" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5056,7 +5085,7 @@
       <c r="B303" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C303" s="11" t="s">
+      <c r="C303" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5067,7 +5096,7 @@
       <c r="B304" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="C304" s="11" t="s">
+      <c r="C304" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5078,7 +5107,7 @@
       <c r="B305" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C305" s="11" t="s">
+      <c r="C305" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5089,7 +5118,7 @@
       <c r="B306" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C306" s="11" t="s">
+      <c r="C306" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5100,7 +5129,7 @@
       <c r="B307" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C307" s="11" t="s">
+      <c r="C307" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5111,7 +5140,7 @@
       <c r="B308" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="C308" s="11" t="s">
+      <c r="C308" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5122,7 +5151,7 @@
       <c r="B309" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C309" s="11" t="s">
+      <c r="C309" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5133,7 +5162,7 @@
       <c r="B310" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C310" s="11" t="s">
+      <c r="C310" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5144,7 +5173,7 @@
       <c r="B311" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C311" s="11" t="s">
+      <c r="C311" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5155,7 +5184,7 @@
       <c r="B312" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C312" s="11" t="s">
+      <c r="C312" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5166,7 +5195,7 @@
       <c r="B313" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C313" s="11" t="s">
+      <c r="C313" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5177,7 +5206,7 @@
       <c r="B314" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C314" s="11" t="s">
+      <c r="C314" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5188,7 +5217,7 @@
       <c r="B315" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C315" s="11" t="s">
+      <c r="C315" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5199,7 +5228,7 @@
       <c r="B316" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C316" s="11" t="s">
+      <c r="C316" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5210,7 +5239,7 @@
       <c r="B317" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C317" s="11" t="s">
+      <c r="C317" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5221,7 +5250,7 @@
       <c r="B318" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C318" s="11" t="s">
+      <c r="C318" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5232,7 +5261,7 @@
       <c r="B319" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="C319" s="11" t="s">
+      <c r="C319" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5243,7 +5272,7 @@
       <c r="B320" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C320" s="11" t="s">
+      <c r="C320" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5254,7 +5283,7 @@
       <c r="B321" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="C321" s="11" t="s">
+      <c r="C321" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5265,7 +5294,7 @@
       <c r="B322" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C322" s="11" t="s">
+      <c r="C322" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5276,7 +5305,7 @@
       <c r="B323" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C323" s="11" t="s">
+      <c r="C323" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5287,7 +5316,7 @@
       <c r="B324" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="C324" s="11" t="s">
+      <c r="C324" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5298,7 +5327,7 @@
       <c r="B325" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="C325" s="11" t="s">
+      <c r="C325" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5309,7 +5338,7 @@
       <c r="B326" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C326" s="11" t="s">
+      <c r="C326" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5320,7 +5349,7 @@
       <c r="B327" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="C327" s="11" t="s">
+      <c r="C327" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5331,7 +5360,7 @@
       <c r="B328" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C328" s="11" t="s">
+      <c r="C328" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5342,7 +5371,7 @@
       <c r="B329" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C329" s="11" t="s">
+      <c r="C329" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5353,7 +5382,7 @@
       <c r="B330" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="C330" s="11" t="s">
+      <c r="C330" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5364,7 +5393,7 @@
       <c r="B331" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="C331" s="11" t="s">
+      <c r="C331" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5375,7 +5404,7 @@
       <c r="B332" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="C332" s="11" t="s">
+      <c r="C332" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5386,17 +5415,17 @@
       <c r="B333" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C333" s="11" t="s">
+      <c r="C333" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="21">
       <c r="B334" s="5"/>
-      <c r="C334" s="11"/>
+      <c r="C334" s="10"/>
     </row>
     <row r="335" spans="1:3" ht="21">
       <c r="B335" s="5"/>
-      <c r="C335" s="11"/>
+      <c r="C335" s="10"/>
     </row>
     <row r="336" spans="1:3" ht="21">
       <c r="A336" s="6" t="s">
@@ -5405,7 +5434,7 @@
       <c r="B336" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C336" s="11" t="s">
+      <c r="C336" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5416,7 +5445,7 @@
       <c r="B337" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C337" s="11" t="s">
+      <c r="C337" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5427,7 +5456,7 @@
       <c r="B338" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="C338" s="11" t="s">
+      <c r="C338" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5438,7 +5467,7 @@
       <c r="B339" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="C339" s="11" t="s">
+      <c r="C339" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5449,7 +5478,7 @@
       <c r="B340" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="C340" s="11" t="s">
+      <c r="C340" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5460,7 +5489,7 @@
       <c r="B341" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C341" s="11" t="s">
+      <c r="C341" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5471,7 +5500,7 @@
       <c r="B342" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="C342" s="11" t="s">
+      <c r="C342" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5482,7 +5511,7 @@
       <c r="B343" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C343" s="11" t="s">
+      <c r="C343" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5493,7 +5522,7 @@
       <c r="B344" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="C344" s="11" t="s">
+      <c r="C344" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5504,7 +5533,7 @@
       <c r="B345" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="C345" s="11" t="s">
+      <c r="C345" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5515,7 +5544,7 @@
       <c r="B346" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="C346" s="11" t="s">
+      <c r="C346" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5526,7 +5555,7 @@
       <c r="B347" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C347" s="11" t="s">
+      <c r="C347" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5537,7 +5566,7 @@
       <c r="B348" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="C348" s="11" t="s">
+      <c r="C348" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5548,7 +5577,7 @@
       <c r="B349" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="C349" s="11" t="s">
+      <c r="C349" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5559,7 +5588,7 @@
       <c r="B350" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="C350" s="11" t="s">
+      <c r="C350" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5570,7 +5599,7 @@
       <c r="B351" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C351" s="11" t="s">
+      <c r="C351" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5581,7 +5610,7 @@
       <c r="B352" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="C352" s="11" t="s">
+      <c r="C352" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5592,17 +5621,17 @@
       <c r="B353" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="C353" s="11" t="s">
+      <c r="C353" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="B354" s="5"/>
-      <c r="C354" s="11"/>
+      <c r="C354" s="10"/>
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="B355" s="5"/>
-      <c r="C355" s="11"/>
+      <c r="C355" s="10"/>
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="6" t="s">
@@ -5611,7 +5640,7 @@
       <c r="B356" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="C356" s="11" t="s">
+      <c r="C356" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5622,7 +5651,7 @@
       <c r="B357" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="C357" s="11" t="s">
+      <c r="C357" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5633,7 +5662,7 @@
       <c r="B358" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="C358" s="11" t="s">
+      <c r="C358" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5644,7 +5673,7 @@
       <c r="B359" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="C359" s="11" t="s">
+      <c r="C359" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5655,7 +5684,7 @@
       <c r="B360" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="C360" s="11" t="s">
+      <c r="C360" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5666,7 +5695,7 @@
       <c r="B361" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C361" s="11" t="s">
+      <c r="C361" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5677,7 +5706,7 @@
       <c r="B362" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="C362" s="11" t="s">
+      <c r="C362" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5688,7 +5717,7 @@
       <c r="B363" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="C363" s="11" t="s">
+      <c r="C363" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5699,7 +5728,7 @@
       <c r="B364" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C364" s="11" t="s">
+      <c r="C364" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5710,7 +5739,7 @@
       <c r="B365" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="C365" s="11" t="s">
+      <c r="C365" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5721,7 +5750,7 @@
       <c r="B366" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C366" s="11" t="s">
+      <c r="C366" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5732,7 +5761,7 @@
       <c r="B367" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C367" s="11" t="s">
+      <c r="C367" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5743,7 +5772,7 @@
       <c r="B368" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C368" s="11" t="s">
+      <c r="C368" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5754,7 +5783,7 @@
       <c r="B369" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C369" s="11" t="s">
+      <c r="C369" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5765,7 +5794,7 @@
       <c r="B370" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C370" s="11" t="s">
+      <c r="C370" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5776,7 +5805,7 @@
       <c r="B371" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="C371" s="11" t="s">
+      <c r="C371" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5787,7 +5816,7 @@
       <c r="B372" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C372" s="11" t="s">
+      <c r="C372" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5798,7 +5827,7 @@
       <c r="B373" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="C373" s="11" t="s">
+      <c r="C373" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5809,7 +5838,7 @@
       <c r="B374" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C374" s="11" t="s">
+      <c r="C374" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5820,7 +5849,7 @@
       <c r="B375" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C375" s="11" t="s">
+      <c r="C375" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5831,7 +5860,7 @@
       <c r="B376" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C376" s="11" t="s">
+      <c r="C376" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5842,7 +5871,7 @@
       <c r="B377" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="C377" s="11" t="s">
+      <c r="C377" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5853,7 +5882,7 @@
       <c r="B378" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C378" s="11" t="s">
+      <c r="C378" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5864,7 +5893,7 @@
       <c r="B379" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C379" s="11" t="s">
+      <c r="C379" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5875,7 +5904,7 @@
       <c r="B380" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C380" s="11" t="s">
+      <c r="C380" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5886,7 +5915,7 @@
       <c r="B381" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="C381" s="11" t="s">
+      <c r="C381" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5897,7 +5926,7 @@
       <c r="B382" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C382" s="11" t="s">
+      <c r="C382" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5908,7 +5937,7 @@
       <c r="B383" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="C383" s="11" t="s">
+      <c r="C383" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5919,7 +5948,7 @@
       <c r="B384" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="C384" s="11" t="s">
+      <c r="C384" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5930,7 +5959,7 @@
       <c r="B385" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="C385" s="11" t="s">
+      <c r="C385" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5941,7 +5970,7 @@
       <c r="B386" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C386" s="11" t="s">
+      <c r="C386" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5952,7 +5981,7 @@
       <c r="B387" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="C387" s="11" t="s">
+      <c r="C387" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5963,7 +5992,7 @@
       <c r="B388" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="C388" s="11" t="s">
+      <c r="C388" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5974,7 +6003,7 @@
       <c r="B389" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C389" s="11" t="s">
+      <c r="C389" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5985,7 +6014,7 @@
       <c r="B390" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C390" s="11" t="s">
+      <c r="C390" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5996,7 +6025,7 @@
       <c r="B391" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="C391" s="11" t="s">
+      <c r="C391" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6007,7 +6036,7 @@
       <c r="B392" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C392" s="11" t="s">
+      <c r="C392" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6018,7 +6047,7 @@
       <c r="B393" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="C393" s="11" t="s">
+      <c r="C393" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6029,7 +6058,7 @@
       <c r="B394" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C394" s="11" t="s">
+      <c r="C394" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6040,7 +6069,7 @@
       <c r="B395" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C395" s="11" t="s">
+      <c r="C395" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6051,7 +6080,7 @@
       <c r="B396" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="C396" s="11" t="s">
+      <c r="C396" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6062,7 +6091,7 @@
       <c r="B397" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C397" s="11" t="s">
+      <c r="C397" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6073,7 +6102,7 @@
       <c r="B398" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="C398" s="11" t="s">
+      <c r="C398" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6084,17 +6113,17 @@
       <c r="B399" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="C399" s="11" t="s">
+      <c r="C399" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="B400" s="5"/>
-      <c r="C400" s="11"/>
+      <c r="C400" s="10"/>
     </row>
     <row r="401" spans="1:3" ht="21">
       <c r="B401" s="5"/>
-      <c r="C401" s="11"/>
+      <c r="C401" s="10"/>
     </row>
     <row r="402" spans="1:3" ht="21">
       <c r="A402" s="6" t="s">
@@ -6103,7 +6132,7 @@
       <c r="B402" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C402" s="11" t="s">
+      <c r="C402" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6114,7 +6143,7 @@
       <c r="B403" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="C403" s="11" t="s">
+      <c r="C403" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6125,7 +6154,7 @@
       <c r="B404" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="C404" s="11" t="s">
+      <c r="C404" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6136,7 +6165,7 @@
       <c r="B405" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C405" s="11" t="s">
+      <c r="C405" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6147,7 +6176,7 @@
       <c r="B406" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C406" s="11" t="s">
+      <c r="C406" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6158,17 +6187,17 @@
       <c r="B407" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="C407" s="11" t="s">
+      <c r="C407" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="B408" s="5"/>
-      <c r="C408" s="11"/>
+      <c r="C408" s="10"/>
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="B409" s="5"/>
-      <c r="C409" s="11"/>
+      <c r="C409" s="10"/>
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="3" t="s">
@@ -6177,7 +6206,7 @@
       <c r="B410" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C410" s="11" t="s">
+      <c r="C410" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6188,7 +6217,7 @@
       <c r="B411" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C411" s="11" t="s">
+      <c r="C411" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6199,7 +6228,7 @@
       <c r="B412" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="C412" s="11" t="s">
+      <c r="C412" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6210,7 +6239,7 @@
       <c r="B413" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C413" s="11" t="s">
+      <c r="C413" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6221,7 +6250,7 @@
       <c r="B414" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C414" s="11" t="s">
+      <c r="C414" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6232,7 +6261,7 @@
       <c r="B415" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C415" s="11" t="s">
+      <c r="C415" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6243,7 +6272,7 @@
       <c r="B416" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="C416" s="11" t="s">
+      <c r="C416" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6254,7 +6283,7 @@
       <c r="B417" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C417" s="11" t="s">
+      <c r="C417" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6265,7 +6294,7 @@
       <c r="B418" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="C418" s="11" t="s">
+      <c r="C418" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6276,7 +6305,7 @@
       <c r="B419" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="C419" s="11" t="s">
+      <c r="C419" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6287,7 +6316,7 @@
       <c r="B420" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="C420" s="11" t="s">
+      <c r="C420" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6298,7 +6327,7 @@
       <c r="B421" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="C421" s="11" t="s">
+      <c r="C421" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6309,7 +6338,7 @@
       <c r="B422" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="C422" s="11" t="s">
+      <c r="C422" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6320,7 +6349,7 @@
       <c r="B423" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="C423" s="11" t="s">
+      <c r="C423" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6331,7 +6360,7 @@
       <c r="B424" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="C424" s="11" t="s">
+      <c r="C424" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6342,7 +6371,7 @@
       <c r="B425" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C425" s="11" t="s">
+      <c r="C425" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6353,7 +6382,7 @@
       <c r="B426" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="C426" s="11" t="s">
+      <c r="C426" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6364,7 +6393,7 @@
       <c r="B427" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="C427" s="11" t="s">
+      <c r="C427" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6375,7 +6404,7 @@
       <c r="B428" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C428" s="11" t="s">
+      <c r="C428" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6386,7 +6415,7 @@
       <c r="B429" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C429" s="11" t="s">
+      <c r="C429" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6397,7 +6426,7 @@
       <c r="B430" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="C430" s="11" t="s">
+      <c r="C430" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6408,7 +6437,7 @@
       <c r="B431" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="C431" s="11" t="s">
+      <c r="C431" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6419,7 +6448,7 @@
       <c r="B432" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="C432" s="11" t="s">
+      <c r="C432" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6430,7 +6459,7 @@
       <c r="B433" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C433" s="11" t="s">
+      <c r="C433" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6441,7 +6470,7 @@
       <c r="B434" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C434" s="11" t="s">
+      <c r="C434" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6452,7 +6481,7 @@
       <c r="B435" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C435" s="11" t="s">
+      <c r="C435" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6463,7 +6492,7 @@
       <c r="B436" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="C436" s="11" t="s">
+      <c r="C436" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6474,7 +6503,7 @@
       <c r="B437" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="C437" s="11" t="s">
+      <c r="C437" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6485,7 +6514,7 @@
       <c r="B438" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="C438" s="11" t="s">
+      <c r="C438" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6496,7 +6525,7 @@
       <c r="B439" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="C439" s="11" t="s">
+      <c r="C439" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6507,7 +6536,7 @@
       <c r="B440" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="C440" s="11" t="s">
+      <c r="C440" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6518,7 +6547,7 @@
       <c r="B441" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="C441" s="11" t="s">
+      <c r="C441" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6529,7 +6558,7 @@
       <c r="B442" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="C442" s="11" t="s">
+      <c r="C442" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6540,7 +6569,7 @@
       <c r="B443" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="C443" s="11" t="s">
+      <c r="C443" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6551,7 +6580,7 @@
       <c r="B444" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="C444" s="11" t="s">
+      <c r="C444" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6562,7 +6591,7 @@
       <c r="B445" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="C445" s="11" t="s">
+      <c r="C445" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6573,7 +6602,7 @@
       <c r="B446" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="C446" s="11" t="s">
+      <c r="C446" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6584,7 +6613,7 @@
       <c r="B447" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C447" s="11" t="s">
+      <c r="C447" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6595,7 +6624,7 @@
       <c r="B448" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="C448" s="11" t="s">
+      <c r="C448" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6606,7 +6635,7 @@
       <c r="B449" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="C449" s="11" t="s">
+      <c r="C449" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6617,7 +6646,7 @@
       <c r="B450" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="C450" s="11" t="s">
+      <c r="C450" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6628,7 +6657,7 @@
       <c r="B451" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="C451" s="11" t="s">
+      <c r="C451" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6639,7 +6668,7 @@
       <c r="B452" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="C452" s="11" t="s">
+      <c r="C452" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6650,7 +6679,7 @@
       <c r="B453" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="C453" s="11" t="s">
+      <c r="C453" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6661,7 +6690,7 @@
       <c r="B454" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="C454" s="11" t="s">
+      <c r="C454" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6672,7 +6701,7 @@
       <c r="B455" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="C455" s="11" t="s">
+      <c r="C455" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6683,7 +6712,7 @@
       <c r="B456" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="C456" s="11" t="s">
+      <c r="C456" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6694,7 +6723,7 @@
       <c r="B457" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="C457" s="11" t="s">
+      <c r="C457" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6705,7 +6734,7 @@
       <c r="B458" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="C458" s="11" t="s">
+      <c r="C458" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6716,7 +6745,7 @@
       <c r="B459" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="C459" s="11" t="s">
+      <c r="C459" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6727,7 +6756,7 @@
       <c r="B460" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="C460" s="11" t="s">
+      <c r="C460" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6738,7 +6767,7 @@
       <c r="B461" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="C461" s="11" t="s">
+      <c r="C461" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6749,7 +6778,7 @@
       <c r="B462" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="C462" s="11" t="s">
+      <c r="C462" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6760,7 +6789,7 @@
       <c r="B463" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="C463" s="11" t="s">
+      <c r="C463" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6771,7 +6800,7 @@
       <c r="B464" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="C464" s="11" t="s">
+      <c r="C464" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6782,7 +6811,7 @@
       <c r="B465" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="C465" s="11" t="s">
+      <c r="C465" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6793,7 +6822,7 @@
       <c r="B466" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="C466" s="11" t="s">
+      <c r="C466" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6804,7 +6833,7 @@
       <c r="B467" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="C467" s="11" t="s">
+      <c r="C467" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6815,7 +6844,7 @@
       <c r="B468" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="C468" s="11" t="s">
+      <c r="C468" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6826,18 +6855,18 @@
       <c r="B469" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="C469" s="11" t="s">
+      <c r="C469" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="B470" s="5"/>
-      <c r="C470" s="11"/>
+      <c r="C470" s="10"/>
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="6"/>
       <c r="B471" s="5"/>
-      <c r="C471" s="11"/>
+      <c r="C471" s="10"/>
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="3" t="s">
@@ -6846,7 +6875,7 @@
       <c r="B472" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="C472" s="11" t="s">
+      <c r="C472" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6857,7 +6886,7 @@
       <c r="B473" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="C473" s="11" t="s">
+      <c r="C473" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6868,7 +6897,7 @@
       <c r="B474" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="C474" s="11" t="s">
+      <c r="C474" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6879,7 +6908,7 @@
       <c r="B475" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="C475" s="11" t="s">
+      <c r="C475" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6890,7 +6919,7 @@
       <c r="B476" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="C476" s="11" t="s">
+      <c r="C476" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6901,7 +6930,7 @@
       <c r="B477" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="C477" s="11" t="s">
+      <c r="C477" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6912,7 +6941,7 @@
       <c r="B478" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="C478" s="11" t="s">
+      <c r="C478" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6923,7 +6952,7 @@
       <c r="B479" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="C479" s="11" t="s">
+      <c r="C479" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6934,7 +6963,7 @@
       <c r="B480" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="C480" s="11" t="s">
+      <c r="C480" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6945,7 +6974,7 @@
       <c r="B481" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="C481" s="11" t="s">
+      <c r="C481" s="10" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>